<commit_message>
Final update on the optimization paramters sheets of these files
</commit_message>
<xml_diff>
--- a/test_files/perturbation_tests/to_be_reformatted/seaver_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test10_output.xlsx
+++ b/test_files/perturbation_tests/to_be_reformatted/seaver_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test10_output.xlsx
@@ -2480,7 +2480,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2556,7 +2556,9 @@
       <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">

</xml_diff>